<commit_message>
feat(Hx): modelo fisico primeras tres h1
</commit_message>
<xml_diff>
--- a/modelos/bitacora_iteraciones_template.xlsx
+++ b/modelos/bitacora_iteraciones_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\bici-go-bd\modelos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USAURIO\bici-go-bd\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF0B629-94D2-411B-A4C0-0BA72C851B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B91FBC-0E5C-4521-8F07-40715EAA6B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitacora" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Iteración</t>
   </si>
@@ -134,6 +134,27 @@
   </si>
   <si>
     <t>modelos/conceptual/h1</t>
+  </si>
+  <si>
+    <t>feature/modelo_fisico_iteracion_1</t>
+  </si>
+  <si>
+    <t>fisico</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Dilan Linero</t>
+  </si>
+  <si>
+    <t>Creacion modelo fisico de primeras 3 historias</t>
+  </si>
+  <si>
+    <t>v0.4-iter1-fisico</t>
+  </si>
+  <si>
+    <t>modelos/fisico</t>
   </si>
 </sst>
 </file>
@@ -549,30 +570,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="57.6640625" customWidth="1"/>
-    <col min="10" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="42.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="57.7109375" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="42.7109375" customWidth="1"/>
     <col min="13" max="13" width="81" customWidth="1"/>
-    <col min="14" max="14" width="78.5546875" customWidth="1"/>
+    <col min="14" max="14" width="78.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +635,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -655,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -696,7 +717,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -735,6 +756,44 @@
       </c>
       <c r="M4" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="3">
+        <v>45939</v>
+      </c>
+      <c r="K5" s="3">
+        <v>45941</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglo, detalles de primera iteracion
</commit_message>
<xml_diff>
--- a/modelos/bitacora_iteraciones_template.xlsx
+++ b/modelos/bitacora_iteraciones_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USAURIO\bici-go-bd\modelos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\bici-go-bd\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B91FBC-0E5C-4521-8F07-40715EAA6B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57AD03D-56E4-4261-82A4-97ECDFECC21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitacora" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Iteración</t>
   </si>
@@ -155,6 +155,27 @@
   </si>
   <si>
     <t>modelos/fisico</t>
+  </si>
+  <si>
+    <t>https://github.com/andr4f/bici-go-bd/pull/10/commits/87b1ee228cea42e67d90cb52a9d8612d7fdee552</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>conceptual,logico,fisico,creacion</t>
+  </si>
+  <si>
+    <t>https://github.com/andr4f/bici-go-bd/pull/11</t>
+  </si>
+  <si>
+    <t>v0.5-iter1-fisico</t>
+  </si>
+  <si>
+    <t>Merge a main de primeras 3 historias</t>
+  </si>
+  <si>
+    <t>bici_go_bd</t>
   </si>
 </sst>
 </file>
@@ -224,13 +245,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -570,30 +592,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="57.7109375" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="57.6640625" customWidth="1"/>
+    <col min="10" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="42.6640625" customWidth="1"/>
     <col min="13" max="13" width="81" customWidth="1"/>
-    <col min="14" max="14" width="78.5703125" customWidth="1"/>
+    <col min="14" max="14" width="78.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +657,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -676,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -717,7 +739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -758,7 +780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -777,6 +799,9 @@
       <c r="F5" t="s">
         <v>41</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="H5" t="s">
         <v>43</v>
       </c>
@@ -794,11 +819,54 @@
       </c>
       <c r="M5" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45942</v>
+      </c>
+      <c r="K6" s="4">
+        <v>45942</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{3B7A025C-D54F-423D-8940-9A69AB9B1AA0}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{02D14F77-4C92-4034-BDA2-19B8ACA38146}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{B4CEFF8D-DDDE-4135-86C8-D93E07F2D697}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>